<commit_message>
add randomizer and updated xlsx
</commit_message>
<xml_diff>
--- a/superbowl_squares.xlsx
+++ b/superbowl_squares.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sejaldua/Desktop/misc/superbowl-squares/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34185C7B-9A6C-F944-8C7E-5DC2D8F6806C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E17B3D5-4E21-5C42-836C-799FD3E1D22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16500"/>
+    <workbookView xWindow="38960" yWindow="-21100" windowWidth="28040" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="superbowl_squares" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -919,16 +919,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -947,34 +948,34 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
+      <c r="L2">
         <v>8</v>
-      </c>
-      <c r="L2">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -982,7 +983,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1018,7 +1019,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1054,7 +1055,7 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1090,7 +1091,7 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1126,7 +1127,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1162,7 +1163,7 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1198,7 +1199,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -1234,7 +1235,7 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -1270,7 +1271,7 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>

</xml_diff>